<commit_message>
Aula 13Mar - 2134
</commit_message>
<xml_diff>
--- a/docs/class_2702.xlsx
+++ b/docs/class_2702.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
   <si>
     <t>endereço de ip</t>
   </si>
@@ -157,6 +157,42 @@
   </si>
   <si>
     <t>PROTOCOLOS</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>\0</t>
+  </si>
+  <si>
+    <t>char</t>
+  </si>
+  <si>
+    <t>( inteiro de 1 B )</t>
+  </si>
+  <si>
+    <t>href;target;caption</t>
   </si>
 </sst>
 </file>
@@ -336,6 +372,10 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -351,10 +391,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2871,29 +2907,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:AE14"/>
+  <dimension ref="C2:AS22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13:J13"/>
+      <selection activeCell="V21" sqref="V21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="17" max="25" width="3" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C3" s="7"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
-      <c r="F3" s="9"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13"/>
     </row>
     <row r="4" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="N5" s="7">
+      <c r="N5" s="11">
         <v>10</v>
       </c>
-      <c r="O5" s="8"/>
-      <c r="P5" s="8"/>
-      <c r="Q5" s="9"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="12"/>
+      <c r="Q5" s="13"/>
       <c r="S5" t="s">
         <v>3</v>
       </c>
@@ -2907,20 +2946,20 @@
     </row>
     <row r="12" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="3:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G13" s="7"/>
-      <c r="H13" s="8"/>
-      <c r="I13" s="8"/>
-      <c r="J13" s="9"/>
-      <c r="K13" s="7">
+      <c r="G13" s="11"/>
+      <c r="H13" s="12"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="11">
         <v>25</v>
       </c>
-      <c r="L13" s="8"/>
-      <c r="M13" s="8"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
-      <c r="Q13" s="8"/>
-      <c r="R13" s="9"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="12"/>
+      <c r="N13" s="13"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="12"/>
+      <c r="Q13" s="12"/>
+      <c r="R13" s="13"/>
       <c r="T13" t="s">
         <v>5</v>
       </c>
@@ -2937,6 +2976,138 @@
       </c>
       <c r="O14">
         <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="7:45" x14ac:dyDescent="0.25">
+      <c r="AP18" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="21" spans="7:45" x14ac:dyDescent="0.25">
+      <c r="G21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="J21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="K21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="L21" s="8"/>
+      <c r="M21" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="N21" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="O21" s="8"/>
+      <c r="P21" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q21" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="R21" s="8" t="s">
+        <v>46</v>
+      </c>
+      <c r="S21" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="T21" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="U21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="V21" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="W21" s="8"/>
+      <c r="X21" s="8"/>
+      <c r="Y21" s="8"/>
+      <c r="Z21" s="8"/>
+      <c r="AA21" s="8"/>
+      <c r="AB21" s="8"/>
+      <c r="AC21" s="8"/>
+      <c r="AD21" s="8"/>
+      <c r="AE21" s="8"/>
+      <c r="AF21" s="8"/>
+      <c r="AG21" s="8"/>
+      <c r="AH21" s="8"/>
+      <c r="AI21" s="8"/>
+      <c r="AJ21" s="8"/>
+      <c r="AK21" s="8"/>
+      <c r="AL21" s="8"/>
+    </row>
+    <row r="22" spans="7:45" x14ac:dyDescent="0.25">
+      <c r="G22">
+        <v>0</v>
+      </c>
+      <c r="H22">
+        <v>1</v>
+      </c>
+      <c r="I22">
+        <v>2</v>
+      </c>
+      <c r="J22">
+        <v>3</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+      <c r="L22">
+        <v>5</v>
+      </c>
+      <c r="M22">
+        <v>6</v>
+      </c>
+      <c r="N22">
+        <v>7</v>
+      </c>
+      <c r="O22">
+        <v>8</v>
+      </c>
+      <c r="P22">
+        <v>9</v>
+      </c>
+      <c r="Q22">
+        <v>10</v>
+      </c>
+      <c r="R22">
+        <v>11</v>
+      </c>
+      <c r="S22">
+        <v>12</v>
+      </c>
+      <c r="T22">
+        <v>13</v>
+      </c>
+      <c r="U22">
+        <v>14</v>
+      </c>
+      <c r="V22">
+        <v>15</v>
+      </c>
+      <c r="W22">
+        <v>16</v>
+      </c>
+      <c r="X22">
+        <v>17</v>
+      </c>
+      <c r="Y22">
+        <v>18</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -3123,8 +3294,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3194,7 +3365,7 @@
       <c r="I4" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10">
+      <c r="A8" s="14">
         <v>0</v>
       </c>
       <c r="B8" s="5"/>
@@ -3207,9 +3378,12 @@
       <c r="E8" s="6" t="s">
         <v>33</v>
       </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10"/>
+      <c r="A9" s="14"/>
       <c r="B9" s="6">
         <v>0</v>
       </c>
@@ -3218,7 +3392,7 @@
       <c r="E9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10"/>
+      <c r="A10" s="14"/>
       <c r="B10" s="6">
         <v>1</v>
       </c>
@@ -3227,7 +3401,7 @@
       <c r="E10" s="5"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="6">
         <v>2</v>
       </c>
@@ -3236,7 +3410,7 @@
       <c r="E11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="11">
+      <c r="A12" s="15">
         <v>1</v>
       </c>
       <c r="B12" s="4"/>
@@ -3251,7 +3425,7 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="11"/>
+      <c r="A13" s="15"/>
       <c r="B13" s="3">
         <v>0</v>
       </c>
@@ -3260,7 +3434,7 @@
       <c r="E13" s="4"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="11"/>
+      <c r="A14" s="15"/>
       <c r="B14" s="3">
         <v>1</v>
       </c>
@@ -3269,7 +3443,7 @@
       <c r="E14" s="4"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="11"/>
+      <c r="A15" s="15"/>
       <c r="B15" s="3">
         <v>2</v>
       </c>
@@ -3278,7 +3452,7 @@
       <c r="E15" s="4"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="10">
+      <c r="A16" s="14">
         <v>2</v>
       </c>
       <c r="B16" s="5"/>
@@ -3293,7 +3467,7 @@
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="10"/>
+      <c r="A17" s="14"/>
       <c r="B17" s="6">
         <v>0</v>
       </c>
@@ -3302,7 +3476,7 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="10"/>
+      <c r="A18" s="14"/>
       <c r="B18" s="6">
         <v>1</v>
       </c>
@@ -3311,7 +3485,7 @@
       <c r="E18" s="5"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="10"/>
+      <c r="A19" s="14"/>
       <c r="B19" s="6">
         <v>2</v>
       </c>
@@ -3334,7 +3508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -3373,9 +3547,9 @@
       <c r="C5" t="s">
         <v>36</v>
       </c>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
+      <c r="H5" s="7"/>
+      <c r="I5" s="7"/>
+      <c r="J5" s="7"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
@@ -3384,9 +3558,9 @@
       <c r="C6" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="13"/>
-      <c r="I6" s="13"/>
-      <c r="J6" s="13"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -3395,49 +3569,49 @@
       <c r="C7" t="s">
         <v>38</v>
       </c>
-      <c r="H7" s="14"/>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14"/>
+      <c r="H7" s="9"/>
+      <c r="I7" s="9"/>
+      <c r="J7" s="9"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H10" s="15"/>
-      <c r="I10" s="15"/>
-      <c r="J10" s="15"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H11" s="15"/>
-      <c r="I11" s="15"/>
-      <c r="J11" s="15"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H12" s="15"/>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="J12" s="10"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H13" s="15"/>
-      <c r="I13" s="15"/>
-      <c r="J13" s="15"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="10"/>
+      <c r="J13" s="10"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H14" s="15"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
+      <c r="H14" s="10"/>
+      <c r="I14" s="10"/>
+      <c r="J14" s="10"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="H15" s="15"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="10"/>
+      <c r="J15" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Aula 20/Mar - herança e autoload
</commit_message>
<xml_diff>
--- a/docs/class_2702.xlsx
+++ b/docs/class_2702.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7755" firstSheet="1" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Plan5" sheetId="6" r:id="rId6"/>
     <sheet name="Plan6" sheetId="7" r:id="rId7"/>
     <sheet name="Plan7" sheetId="8" r:id="rId8"/>
+    <sheet name="Plan8" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="60">
   <si>
     <t>endereço de ip</t>
   </si>
@@ -193,13 +194,31 @@
   </si>
   <si>
     <t>href;target;caption</t>
+  </si>
+  <si>
+    <t>stack __autoload</t>
+  </si>
+  <si>
+    <t>é uma tabela</t>
+  </si>
+  <si>
+    <t>cada linha na tabela mapeia uma função que será executada quando eu tentar criar</t>
+  </si>
+  <si>
+    <t>um objeto de uma classe que não foi definida no script em execução</t>
+  </si>
+  <si>
+    <t>loader</t>
+  </si>
+  <si>
+    <t>abacaxi</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -209,6 +228,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -360,7 +387,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
@@ -391,6 +418,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3294,7 +3322,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3616,4 +3644,47 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A3:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G15" s="16"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>